<commit_message>
Featured added to invoke methods Dynamically
</commit_message>
<xml_diff>
--- a/Run Manager.xlsx
+++ b/Run Manager.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Info" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Test Case Desc</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Test@123!</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>LoginPageTest</t>
   </si>
 </sst>
 </file>
@@ -395,11 +401,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -410,37 +414,43 @@
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -453,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added WebView handling capability
</commit_message>
<xml_diff>
--- a/Run Manager.xlsx
+++ b/Run Manager.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Test Case Desc</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Chrome</t>
   </si>
   <si>
-    <t>iOS</t>
-  </si>
-  <si>
     <t>User Name</t>
   </si>
   <si>
@@ -76,6 +73,12 @@
   </si>
   <si>
     <t>LoginPageTest</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
 </sst>
 </file>
@@ -401,9 +404,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -416,7 +421,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -436,7 +441,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -451,7 +456,27 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -464,7 +489,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,10 +504,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -490,10 +515,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>